<commit_message>
Deleteing and adding Excel file as per workflow
</commit_message>
<xml_diff>
--- a/Feedback-Triggered-Certificate-Bot/Maillist.xlsx
+++ b/Feedback-Triggered-Certificate-Bot/Maillist.xlsx
@@ -1,104 +1,121 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="510" yWindow="630" windowWidth="14055" windowHeight="4050"/>
-  </bookViews>
-  <sheets>
-    <sheet name="MailList" sheetId="2" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="125725"/>
-</workbook>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:workbookPr codeName="ThisWorkbook"/>
+  <x:bookViews>
+    <x:workbookView firstSheet="0" activeTab="0"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="MailList" sheetId="2" r:id="rId2"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="125725"/>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Google Cloud Support</t>
-  </si>
-  <si>
-    <t>certification-support@feedback.google.com</t>
-  </si>
-  <si>
-    <t>Alumni Coordinator at AlmaConnect</t>
-  </si>
-  <si>
-    <t>member@almaconnect.email</t>
-  </si>
-  <si>
-    <t>Flipkart.com</t>
-  </si>
-  <si>
-    <t>no-reply@flipkart.com</t>
-  </si>
-  <si>
-    <t>Reddit</t>
-  </si>
-  <si>
-    <t>noreply@redditmail.com</t>
-  </si>
-  <si>
-    <t>Feedback redBus</t>
-  </si>
-  <si>
-    <t>no_reply_feedback@redbus.in</t>
-  </si>
-  <si>
-    <t>redbus</t>
-  </si>
-  <si>
-    <t>greetings@travel.e-redbus.in</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <x:si>
+    <x:t>Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Email</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Google Cloud Support</x:t>
+  </x:si>
+  <x:si>
+    <x:t>certification-support@feedback.google.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Alumni Coordinator at AlmaConnect</x:t>
+  </x:si>
+  <x:si>
+    <x:t>member@almaconnect.email</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Flipkart.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>no-reply@flipkart.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Reddit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>noreply@redditmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Feedback redBus</x:t>
+  </x:si>
+  <x:si>
+    <x:t>no_reply_feedback@redbus.in</x:t>
+  </x:si>
+  <x:si>
+    <x:t>redbus</x:t>
+  </x:si>
+  <x:si>
+    <x:t>greetings@travel.e-redbus.in</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-</styleSheet>
+<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="1">
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border diagonalUp="0" diagonalDown="0">
+      <x:left style="none">
+        <x:color rgb="FF000000"/>
+      </x:left>
+      <x:right style="none">
+        <x:color rgb="FF000000"/>
+      </x:right>
+      <x:top style="none">
+        <x:color rgb="FF000000"/>
+      </x:top>
+      <x:bottom style="none">
+        <x:color rgb="FF000000"/>
+      </x:bottom>
+      <x:diagonal style="none">
+        <x:color rgb="FF000000"/>
+      </x:diagonal>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,75 +402,77 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="39.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:B7"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:2">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:2">
+      <x:c r="A2" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:2">
+      <x:c r="A3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:2">
+      <x:c r="A4" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:2">
+      <x:c r="A5" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:2">
+      <x:c r="A6" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:2">
+      <x:c r="A7" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>